<commit_message>
updated lots of different things for testing, xls & ssm file generation. Fixed .ssm read_prob to account for X/Y chromosome.
</commit_message>
<xml_diff>
--- a/data/example/example.aggregated.xlsx
+++ b/data/example/example.aggregated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,10 +483,10 @@
         <v>500</v>
       </c>
       <c r="D2" t="n">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -515,10 +515,10 @@
         <v>127</v>
       </c>
       <c r="D3" t="n">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -547,10 +547,10 @@
         <v>502</v>
       </c>
       <c r="D4" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -572,29 +572,29 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>chr10</t>
+          <t>chrY</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>500</v>
+        <v>1043</v>
       </c>
       <c r="D5" t="n">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E5" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Pt0_Er1</t>
+          <t>Pt0_blast</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>chr10_500</t>
+          <t>chrY_1043</t>
         </is>
       </c>
     </row>
@@ -604,17 +604,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>chr9</t>
+          <t>chr10</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>127</v>
+        <v>500</v>
       </c>
       <c r="D6" t="n">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -622,11 +622,11 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.04</v>
+        <v>0.32</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>chr9_127</t>
+          <t>chr10_500</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>chr4</t>
+          <t>chr9</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>502</v>
+        <v>127</v>
       </c>
       <c r="D7" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -654,11 +654,11 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>chr4_502</t>
+          <t>chr9_127</t>
         </is>
       </c>
     </row>
@@ -668,29 +668,29 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>chr10</t>
+          <t>chr4</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D8" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Pt0_NK</t>
+          <t>Pt0_Er1</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>chr10_500</t>
+          <t>chr4_502</t>
         </is>
       </c>
     </row>
@@ -700,29 +700,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>chr9</t>
+          <t>chrY</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>127</v>
+        <v>1043</v>
       </c>
       <c r="D9" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Pt0_NK</t>
+          <t>Pt0_Er1</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>chr9_127</t>
+          <t>chrY_1043</t>
         </is>
       </c>
     </row>
@@ -732,29 +732,253 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>chr10</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>500</v>
+      </c>
+      <c r="D10" t="n">
+        <v>45</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Pt0_NK</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>chr10_500</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>chr9</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>127</v>
+      </c>
+      <c r="D11" t="n">
+        <v>49</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Pt0_NK</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>chr9_127</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>chr4</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C12" t="n">
         <v>502</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D12" t="n">
         <v>44</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E12" t="n">
         <v>6</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>Pt0_NK</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="G12" t="n">
         <v>0.12</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>chr4_502</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>chrY</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1043</v>
+      </c>
+      <c r="D13" t="n">
+        <v>50</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Pt0_NK</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>chrY_1043</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>chr10</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>500</v>
+      </c>
+      <c r="D14" t="n">
+        <v>50</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Pt0_Bcells</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>chr10_500</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>chr9</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>127</v>
+      </c>
+      <c r="D15" t="n">
+        <v>50</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Pt0_Bcells</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>chr9_127</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>chr4</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>502</v>
+      </c>
+      <c r="D16" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Pt0_Bcells</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>chr4_502</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>chrY</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1043</v>
+      </c>
+      <c r="D17" t="n">
+        <v>41</v>
+      </c>
+      <c r="E17" t="n">
+        <v>9</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Pt0_Bcells</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>chrY_1043</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Made updates per request to formatting of .ssm, outputing of metrics, etc.
</commit_message>
<xml_diff>
--- a/data/example/example.aggregated.xlsx
+++ b/data/example/example.aggregated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,11 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>gene</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>chr_pos</t>
         </is>
       </c>
@@ -497,6 +502,11 @@
         <v>0.14</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>chr10_500</t>
         </is>
@@ -530,6 +540,11 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>chr9_127</t>
         </is>
       </c>
@@ -550,7 +565,7 @@
         <v>47</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -561,6 +576,11 @@
         <v>0.06</v>
       </c>
       <c r="H4" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>chr4_502</t>
         </is>
@@ -594,6 +614,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>D1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>chrY_1043</t>
         </is>
       </c>
@@ -626,6 +651,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>chr10_500</t>
         </is>
       </c>
@@ -658,6 +688,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>chr9_127</t>
         </is>
       </c>
@@ -675,7 +710,7 @@
         <v>502</v>
       </c>
       <c r="D8" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -689,6 +724,11 @@
         <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>chr4_502</t>
         </is>
@@ -722,6 +762,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>D1</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>chrY_1043</t>
         </is>
       </c>
@@ -754,6 +799,11 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>chr10_500</t>
         </is>
       </c>
@@ -774,7 +824,7 @@
         <v>49</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -785,6 +835,11 @@
         <v>0.02</v>
       </c>
       <c r="H11" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>chr9_127</t>
         </is>
@@ -818,6 +873,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
           <t>chr4_502</t>
         </is>
       </c>
@@ -850,6 +910,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
+          <t>D1</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
           <t>chrY_1043</t>
         </is>
       </c>
@@ -882,6 +947,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>chr10_500</t>
         </is>
       </c>
@@ -899,7 +969,7 @@
         <v>127</v>
       </c>
       <c r="D15" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -913,6 +983,11 @@
         <v>0</v>
       </c>
       <c r="H15" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>chr9_127</t>
         </is>
@@ -931,7 +1006,7 @@
         <v>502</v>
       </c>
       <c r="D16" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -945,6 +1020,11 @@
         <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>chr4_502</t>
         </is>
@@ -977,6 +1057,11 @@
         <v>0.18</v>
       </c>
       <c r="H17" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>chrY_1043</t>
         </is>

</xml_diff>

<commit_message>
double checked and corrected aggregation metrics. Sorted dataframes by chromosome number.
</commit_message>
<xml_diff>
--- a/data/example/example.aggregated.xlsx
+++ b/data/example/example.aggregated.xlsx
@@ -481,17 +481,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>chr10</t>
+          <t>chrY</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>500</v>
+        <v>1043</v>
       </c>
       <c r="D2" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -499,16 +499,16 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.14</v>
+        <v>0</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>chr10_500</t>
+          <t>chrY_1043</t>
         </is>
       </c>
     </row>
@@ -518,34 +518,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>chr9</t>
+          <t>chrY</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>127</v>
+        <v>1043</v>
       </c>
       <c r="D3" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Pt0_blast</t>
+          <t>Pt0_Er1</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.14</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>chr9_127</t>
+          <t>chrY_1043</t>
         </is>
       </c>
     </row>
@@ -555,34 +555,34 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>chr4</t>
+          <t>chrY</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>502</v>
+        <v>1043</v>
       </c>
       <c r="D4" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Pt0_blast</t>
+          <t>Pt0_NK</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>chr4_502</t>
+          <t>chrY_1043</t>
         </is>
       </c>
     </row>
@@ -599,18 +599,18 @@
         <v>1043</v>
       </c>
       <c r="D5" t="n">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Pt0_blast</t>
+          <t>Pt0_Bcells</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -629,34 +629,34 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>chr10</t>
+          <t>chr4</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D6" t="n">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E6" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Pt0_Er1</t>
+          <t>Pt0_blast</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.32</v>
+        <v>0.06</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>chr10_500</t>
+          <t>chr4_502</t>
         </is>
       </c>
     </row>
@@ -666,17 +666,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>chr9</t>
+          <t>chr4</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>127</v>
+        <v>502</v>
       </c>
       <c r="D7" t="n">
         <v>48</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -684,16 +684,16 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>chr9_127</t>
+          <t>chr4_502</t>
         </is>
       </c>
     </row>
@@ -710,18 +710,18 @@
         <v>502</v>
       </c>
       <c r="D8" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Pt0_Er1</t>
+          <t>Pt0_NK</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -740,21 +740,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>chrY</t>
+          <t>chr4</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1043</v>
+        <v>502</v>
       </c>
       <c r="D9" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Pt0_Er1</t>
+          <t>Pt0_Bcells</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -762,12 +762,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>chrY_1043</t>
+          <t>chr4_502</t>
         </is>
       </c>
     </row>
@@ -777,34 +777,34 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>chr10</t>
+          <t>chr9</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>500</v>
+        <v>127</v>
       </c>
       <c r="D10" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Pt0_NK</t>
+          <t>Pt0_blast</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0.1</v>
+        <v>0.14</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>chr10_500</t>
+          <t>chr9_127</t>
         </is>
       </c>
     </row>
@@ -821,18 +821,18 @@
         <v>127</v>
       </c>
       <c r="D11" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Pt0_NK</t>
+          <t>Pt0_Er1</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -851,17 +851,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>chr4</t>
+          <t>chr9</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>502</v>
+        <v>127</v>
       </c>
       <c r="D12" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -869,16 +869,16 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0.12</v>
+        <v>0.02</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>chr4_502</t>
+          <t>chr9_127</t>
         </is>
       </c>
     </row>
@@ -888,21 +888,21 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>chrY</t>
+          <t>chr9</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1043</v>
+        <v>127</v>
       </c>
       <c r="D13" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Pt0_NK</t>
+          <t>Pt0_Bcells</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -910,12 +910,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>chrY_1043</t>
+          <t>chr9_127</t>
         </is>
       </c>
     </row>
@@ -932,18 +932,18 @@
         <v>500</v>
       </c>
       <c r="D14" t="n">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Pt0_Bcells</t>
+          <t>Pt0_blast</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -962,34 +962,34 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>chr9</t>
+          <t>chr10</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>127</v>
+        <v>500</v>
       </c>
       <c r="D15" t="n">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Pt0_Bcells</t>
+          <t>Pt0_Er1</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>chr9_127</t>
+          <t>chr10_500</t>
         </is>
       </c>
     </row>
@@ -999,34 +999,34 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>chr4</t>
+          <t>chr10</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D16" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Pt0_Bcells</t>
+          <t>Pt0_NK</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>chr4_502</t>
+          <t>chr10_500</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>chrY</t>
+          <t>chr10</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1043</v>
+        <v>500</v>
       </c>
       <c r="D17" t="n">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1054,16 +1054,16 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>chrY_1043</t>
+          <t>chr10_500</t>
         </is>
       </c>
     </row>

</xml_diff>